<commit_message>
Doc: Going to sleep...
</commit_message>
<xml_diff>
--- a/Dokumentacia/Dokumentácia/testovanie.xlsx
+++ b/Dokumentacia/Dokumentácia/testovanie.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="24855" windowHeight="12780"/>
+    <workbookView xWindow="-30" yWindow="0" windowWidth="10530" windowHeight="12780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,41 +16,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Master</t>
   </si>
   <si>
-    <t>sw</t>
-  </si>
-  <si>
-    <t>hw /wo</t>
-  </si>
-  <si>
-    <t>hw /w</t>
-  </si>
-  <si>
-    <t>usnecured</t>
-  </si>
-  <si>
-    <t>Code [b]</t>
-  </si>
-  <si>
-    <t>RO data [b]</t>
-  </si>
-  <si>
-    <t>zi data  [b]</t>
-  </si>
-  <si>
     <t>všetko dokopy /wo</t>
   </si>
   <si>
     <t>Zero Initialezed</t>
   </si>
   <si>
-    <t>RW  [b]</t>
-  </si>
-  <si>
     <t>CODE</t>
   </si>
   <si>
@@ -82,6 +58,78 @@
   </si>
   <si>
     <t>672.42</t>
+  </si>
+  <si>
+    <t>263.05</t>
+  </si>
+  <si>
+    <t>253.65</t>
+  </si>
+  <si>
+    <t>551.71</t>
+  </si>
+  <si>
+    <t>541.84</t>
+  </si>
+  <si>
+    <t>1616.86</t>
+  </si>
+  <si>
+    <t>1659.88</t>
+  </si>
+  <si>
+    <t>nothing</t>
+  </si>
+  <si>
+    <t>1.23,1.4</t>
+  </si>
+  <si>
+    <t>v stadnby</t>
+  </si>
+  <si>
+    <t>Implementácia</t>
+  </si>
+  <si>
+    <t>Typ zabezpečenia</t>
+  </si>
+  <si>
+    <t>bez</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>HW</t>
+  </si>
+  <si>
+    <t>AES128 CBC</t>
+  </si>
+  <si>
+    <t>Metriky</t>
+  </si>
+  <si>
+    <t>Pamäť programu [B]</t>
+  </si>
+  <si>
+    <t>RW  [B]</t>
+  </si>
+  <si>
+    <t>ZI  [B]</t>
+  </si>
+  <si>
+    <t>RO [B]</t>
+  </si>
+  <si>
+    <t>Kód [B]</t>
+  </si>
+  <si>
+    <t>bez zabezpečenia</t>
+  </si>
+  <si>
+    <t>HW bez  parametrov</t>
+  </si>
+  <si>
+    <t>HW s parametrami</t>
   </si>
 </sst>
 </file>
@@ -237,13 +285,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -293,6 +339,33 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -589,268 +662,383 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:O11"/>
+  <dimension ref="A2:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="A3" sqref="A3:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1">
+    <row r="2" spans="1:19" ht="15.75" thickBot="1">
       <c r="E2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="H3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="12">
+      <c r="K3" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="10">
         <v>6944</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>316</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>48</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>5648</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="10">
         <f>B4+C4+D4</f>
         <v>7308</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="3">
         <f>D4+E4</f>
         <v>5696</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="4">
         <f>B4+C4</f>
         <v>7260</v>
       </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="18">
+      <c r="J4" s="16">
         <v>3.7614583333333337E-3</v>
       </c>
-      <c r="K4" s="10">
-        <v>100</v>
-      </c>
-      <c r="L4" s="22">
+      <c r="K4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="21">
         <v>323.99</v>
       </c>
       <c r="M4" s="22">
         <v>308.7</v>
       </c>
       <c r="N4" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" s="21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="12">
+        <v>9</v>
+      </c>
+      <c r="O4" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="R4" s="28">
+        <f>(P4+Q4)/2</f>
+        <v>258.35000000000002</v>
+      </c>
+      <c r="S4" s="19"/>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="10">
         <v>10132</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>1144</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>60</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <v>6044</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="10">
         <f t="shared" ref="F5:F8" si="0">B5+C5+D5</f>
         <v>11336</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="3">
         <f t="shared" ref="G5:G8" si="1">D5+E5</f>
         <v>6104</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="4">
         <f t="shared" ref="H5:H8" si="2">B5+C5</f>
         <v>11276</v>
       </c>
       <c r="I5" s="1"/>
-      <c r="J5" s="18">
+      <c r="J5" s="16">
         <v>7.3715277777777781E-3</v>
       </c>
-      <c r="K5" s="10">
-        <v>120</v>
-      </c>
-      <c r="L5" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" s="22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="12">
+      <c r="K5" s="8">
+        <v>5.6</v>
+      </c>
+      <c r="L5" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="26">
+        <v>663.03</v>
+      </c>
+      <c r="P5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q5" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="R5" s="28">
+        <f t="shared" ref="R5:R6" si="3">(P5+Q5)/2</f>
+        <v>546.77500000000009</v>
+      </c>
+      <c r="S5" s="19"/>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="10">
         <v>16302</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>1370</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>740</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="4">
         <v>7220</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="10">
         <f t="shared" si="0"/>
         <v>18412</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="3">
         <f t="shared" si="1"/>
         <v>7960</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="4">
         <f t="shared" si="2"/>
         <v>17672</v>
       </c>
       <c r="I6" s="1"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="11">
-        <v>100</v>
-      </c>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="12">
+      <c r="J6" s="17"/>
+      <c r="K6" s="9">
+        <v>8</v>
+      </c>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="28">
+        <f t="shared" si="3"/>
+        <v>1638.37</v>
+      </c>
+      <c r="S6" s="19"/>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="10">
         <v>16306</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>11110</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>3124</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="4">
         <v>7220</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="10">
         <f t="shared" si="0"/>
         <v>30540</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="3">
         <f t="shared" si="1"/>
         <v>10344</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="4">
         <f t="shared" si="2"/>
         <v>27416</v>
       </c>
       <c r="I7" s="1"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A8" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="13">
+      <c r="J7" s="17"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A8" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="11">
         <v>19482</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="5">
         <v>2202</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="5">
         <v>752</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="6">
         <v>7392</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="11">
         <f t="shared" si="0"/>
         <v>22436</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="5">
         <f t="shared" si="1"/>
         <v>8144</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="6">
         <f t="shared" si="2"/>
         <v>21684</v>
       </c>
       <c r="I8" s="1"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="J8" s="18"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="J9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9">
+        <v>2.6</v>
+      </c>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+    </row>
+    <row r="10" spans="1:19">
       <c r="B10">
         <v>7444</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="K10" s="27">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+    </row>
+    <row r="11" spans="1:19">
       <c r="B11">
         <f>B10-B4</f>
         <v>500</v>
+      </c>
+      <c r="K11" s="27">
+        <v>3.5</v>
+      </c>
+      <c r="L11" t="s">
+        <v>22</v>
+      </c>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>